<commit_message>
Changes to add write msid in Testdata file.
</commit_message>
<xml_diff>
--- a/TestData/ProductionData.xlsx
+++ b/TestData/ProductionData.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19380" windowHeight="6495"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="19380" windowHeight="6500"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="1" r:id="rId1"/>
     <sheet name="ACC" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="F1:P20"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -415,20 +419,20 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="80" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" customWidth="1"/>
+    <col min="4" max="4" width="78.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.1640625" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -457,7 +461,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -492,7 +496,12 @@
     <hyperlink ref="I2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -502,9 +511,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -514,8 +528,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>